<commit_message>
Admin Terminado falta administrador de configuraciones
</commit_message>
<xml_diff>
--- a/assets/Presupuesto-Nuevo-2016-Arueda.xlsx
+++ b/assets/Presupuesto-Nuevo-2016-Arueda.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25580" windowHeight="13500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16260" windowHeight="13500"/>
   </bookViews>
   <sheets>
     <sheet name="COT04012010" sheetId="14" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t xml:space="preserve">PRECIO </t>
   </si>
@@ -54,15 +54,9 @@
     <t>SEÑOR</t>
   </si>
   <si>
-    <t>Asesorias Técnicas, Mantención y Reparación</t>
-  </si>
-  <si>
     <t>CRISTIAN ARRIAGADA BENITES</t>
   </si>
   <si>
-    <t>Email: callcenter.arueda@gmail.com</t>
-  </si>
-  <si>
     <t>PRECIO</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t>Presupuesto Para realizar mantencion y reparacion maquinas de ejercicios</t>
   </si>
   <si>
-    <t>Máquinas de ejercicios</t>
-  </si>
-  <si>
     <t>Fono: +56956028588</t>
   </si>
   <si>
@@ -97,6 +88,9 @@
   </si>
   <si>
     <t>MARCA</t>
+  </si>
+  <si>
+    <t>Email: atom@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -104,8 +98,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="195" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="200" formatCode="&quot;Santiago&quot;\,\ d\ \ mmmm\ &quot;de&quot;\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;Santiago&quot;\,\ d\ \ mmmm\ &quot;de&quot;\ yyyy"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -341,10 +335,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="195" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="200" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -354,14 +348,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="195" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="195" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="195" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -376,21 +370,21 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="195" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="195" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="195" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="195" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -408,8 +402,8 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="195" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="200" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -470,10 +464,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="195" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="195" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -483,10 +477,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="195" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="195" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -496,6 +490,8 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -508,8 +504,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="195" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,7 +667,7 @@
             <a:rPr lang="es-ES" sz="1500" baseline="0">
               <a:latin typeface="+mn-lt"/>
             </a:rPr>
-            <a:t>Email: callcenter.arueda@gmail.com</a:t>
+            <a:t>Email: atom@gmail.com@gmail.com</a:t>
           </a:r>
           <a:endParaRPr lang="es-ES" sz="1500">
             <a:latin typeface="+mn-lt"/>
@@ -681,74 +675,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1103489</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1290" name="1 Imagen" descr="arueda_2.jpg"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="825500" y="127000"/>
-          <a:ext cx="1803400" cy="1524000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -812,136 +738,80 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>28223</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>68503</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>14112</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>81956</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="522112" y="364836"/>
+          <a:ext cx="3273778" cy="1255231"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>176484</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>959555</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>70555</xdr:rowOff>
     </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="1292" name="Group 17"/>
-        <xdr:cNvGrpSpPr>
-          <a:grpSpLocks/>
-        </xdr:cNvGrpSpPr>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr bwMode="auto">
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="570089" y="5136444"/>
-          <a:ext cx="1322211" cy="261056"/>
-          <a:chOff x="110205000" y="110080800"/>
-          <a:chExt cx="453960" cy="111341"/>
+          <a:off x="493889" y="5115373"/>
+          <a:ext cx="959555" cy="289182"/>
         </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="1293" name="Picture 18"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="110277000" y="110080800"/>
-            <a:ext cx="381960" cy="111341"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-            <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:miter lim="800000"/>
-                <a:headEnd/>
-                <a:tailEnd/>
-              </a14:hiddenLine>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="12" name="WordArt 19"/>
-          <xdr:cNvSpPr>
-            <a:spLocks noChangeArrowheads="1" noChangeShapeType="1" noTextEdit="1"/>
-          </xdr:cNvSpPr>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="110205000" y="110110100"/>
-            <a:ext cx="74624" cy="64461"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-        <xdr:txBody>
-          <a:bodyPr wrap="none" fromWordArt="1">
-            <a:prstTxWarp prst="textPlain">
-              <a:avLst>
-                <a:gd name="adj" fmla="val 50000"/>
-              </a:avLst>
-            </a:prstTxWarp>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr" rtl="0"/>
-            <a:r>
-              <a:rPr lang="es-ES" sz="3600" kern="10" spc="0">
-                <a:ln w="9525" algn="ctr">
-                  <a:solidFill>
-                    <a:srgbClr val="28A328"/>
-                  </a:solidFill>
-                  <a:round/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="28A328"/>
-                </a:solidFill>
-                <a:effectLst/>
-                <a:latin typeface="Arial Black"/>
-              </a:rPr>
-              <a:t>a</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1272,7 +1142,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="106" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1302,9 +1172,7 @@
       <c r="A3" s="14"/>
       <c r="B3" s="9"/>
       <c r="C3" s="41"/>
-      <c r="D3" s="64" t="s">
-        <v>8</v>
-      </c>
+      <c r="D3" s="64"/>
       <c r="E3" s="41"/>
       <c r="F3" s="5"/>
       <c r="G3" s="11"/>
@@ -1314,9 +1182,7 @@
       <c r="A4" s="14"/>
       <c r="B4" s="9"/>
       <c r="C4" s="41"/>
-      <c r="D4" s="64" t="s">
-        <v>19</v>
-      </c>
+      <c r="D4" s="64"/>
       <c r="E4" s="41"/>
       <c r="F4" s="5"/>
       <c r="G4" s="11"/>
@@ -1355,19 +1221,19 @@
       <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="80"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
       <c r="G10" s="11"/>
       <c r="J10" s="5"/>
     </row>
@@ -1472,7 +1338,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="18"/>
@@ -1505,10 +1371,10 @@
     </row>
     <row r="20" spans="1:15" ht="14" x14ac:dyDescent="0.15">
       <c r="B20" s="19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D20" s="21" t="s">
         <v>1</v>
@@ -1517,7 +1383,7 @@
         <v>6</v>
       </c>
       <c r="F20" s="66" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G20" s="67" t="s">
         <v>0</v>
@@ -1553,8 +1419,8 @@
       <c r="B22" s="37"/>
       <c r="C22" s="36"/>
       <c r="D22" s="36"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="83"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="79"/>
       <c r="G22" s="22"/>
       <c r="H22" s="3"/>
       <c r="I22" s="1"/>
@@ -1654,7 +1520,7 @@
     <row r="29" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14"/>
       <c r="B29" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
@@ -1673,7 +1539,7 @@
     </row>
     <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="56" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C31" s="53"/>
       <c r="D31" s="53"/>
@@ -1683,7 +1549,7 @@
     </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="57" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C32" s="53"/>
       <c r="D32" s="53"/>
@@ -1732,7 +1598,7 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B1" s="42" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="43"/>
       <c r="D1" s="48"/>
@@ -1740,7 +1606,7 @@
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B2" s="42" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="43"/>
       <c r="D2" s="48"/>
@@ -1754,7 +1620,7 @@
     </row>
     <row r="4" spans="2:5" ht="39" x14ac:dyDescent="0.15">
       <c r="B4" s="45" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="49"/>
@@ -1768,12 +1634,12 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B6" s="42" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="43"/>
       <c r="D6" s="48"/>
       <c r="E6" s="50" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="14" thickBot="1" x14ac:dyDescent="0.2">
@@ -1784,7 +1650,7 @@
     </row>
     <row r="8" spans="2:5" ht="40" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B8" s="46" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="51"/>

</xml_diff>